<commit_message>
Se incluye en la hoja Equipo el registro para Mónica Angulo
</commit_message>
<xml_diff>
--- a/Tablas.xlsx
+++ b/Tablas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sistemas\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f499dd0fb5abc23a/Desktop/mistionTIC/semana-1-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04CC7954-3B46-4AD4-802F-B304045656D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{04CC7954-3B46-4AD4-802F-B304045656D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3C9C939-1A82-4C21-A775-2DE9CD1EC94B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1068" yWindow="-108" windowWidth="22080" windowHeight="13176" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tablas" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="131">
   <si>
     <t>Id</t>
   </si>
@@ -317,9 +317,6 @@
     <t>La felicidad es un buen libro y una taza de café</t>
   </si>
   <si>
-    <t>Comunicador Social - Periodista de la Universidad de la sabana.  Amplia experiencia en investigación de mercados, análisis de datos, téecnicas dee recolección de inforrmación y diseño de estrategias de planeación estrégicca.</t>
-  </si>
-  <si>
     <t>Café de Nariño</t>
   </si>
   <si>
@@ -446,9 +443,6 @@
     <t>Edgar Orozco Guayara</t>
   </si>
   <si>
-    <t>Técnico en Sistemas y Computaciób - Desarrollador de software durante m´´as de veinte años, astrónomo aficionado, fotógrafo y amante de la ciencia ficción.</t>
-  </si>
-  <si>
     <t>En cada sorbo de café hay una buena idea escondida</t>
   </si>
   <si>
@@ -474,6 +468,24 @@
   </si>
   <si>
     <t>Edgar Orozco</t>
+  </si>
+  <si>
+    <t>Mónica Angulo P</t>
+  </si>
+  <si>
+    <t>Amigos y café, la mejor combinación</t>
+  </si>
+  <si>
+    <t>Técnico en Sistemas y Computación - Desarrollador de software durante más de veinte años, astrónomo aficionado, fotógrafo y amante de la ciencia ficción.</t>
+  </si>
+  <si>
+    <t>Comunicador Social - Periodista de la Universidad de la Sabana.  Amplia experiencia en investigación de mercados, análisis de datos, téecnicas dee recolección de inforrmación y diseño de estrategias de planeación estrégicca.</t>
+  </si>
+  <si>
+    <t>Ingeniera de Sistemas del Politécnico Grancolombiano, con experiencia en desarrollo de software, Gerencia de proyectos y, conocimiento y aplicación de metodologías, modelos y normas de calidad enfocadas en el área TI. (SCRUM, CMMI, ITMARK, ITIL, ISO27000, ISO20000)</t>
+  </si>
+  <si>
+    <t>correo</t>
   </si>
 </sst>
 </file>
@@ -1037,20 +1049,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="11.42578125" style="6"/>
-    <col min="10" max="10" width="13.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="6"/>
+    <col min="1" max="1" width="12.88671875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="11.44140625" style="6"/>
+    <col min="10" max="10" width="13.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.44140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
@@ -1058,7 +1070,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
@@ -1066,7 +1078,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
@@ -1086,7 +1098,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
@@ -1103,7 +1115,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>2</v>
       </c>
@@ -1117,7 +1129,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>4</v>
       </c>
@@ -1131,7 +1143,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>26</v>
       </c>
@@ -1139,7 +1151,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>5</v>
       </c>
@@ -1147,12 +1159,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I12" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>18</v>
       </c>
@@ -1160,7 +1172,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>16</v>
       </c>
@@ -1177,7 +1189,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>0</v>
       </c>
@@ -1197,7 +1209,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>9</v>
       </c>
@@ -1214,7 +1226,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>14</v>
       </c>
@@ -1228,7 +1240,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>2</v>
       </c>
@@ -1242,7 +1254,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
         <v>4</v>
       </c>
@@ -1256,15 +1268,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>26</v>
       </c>
@@ -1272,7 +1284,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
         <v>5</v>
       </c>
@@ -1280,17 +1292,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I24" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I25" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C26" s="6" t="s">
         <v>11</v>
       </c>
@@ -1304,7 +1316,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>19</v>
       </c>
@@ -1318,7 +1330,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
         <v>20</v>
       </c>
@@ -1329,7 +1341,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>0</v>
       </c>
@@ -1343,7 +1355,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
         <v>14</v>
       </c>
@@ -1357,7 +1369,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
         <v>21</v>
       </c>
@@ -1365,7 +1377,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
         <v>23</v>
       </c>
@@ -1373,7 +1385,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
         <v>26</v>
       </c>
@@ -1381,7 +1393,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="12" t="s">
         <v>5</v>
       </c>
@@ -1392,12 +1404,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I35" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I36" s="7" t="s">
         <v>0</v>
       </c>
@@ -1408,7 +1420,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I37" s="9" t="s">
         <v>14</v>
       </c>
@@ -1419,7 +1431,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I38" s="9" t="s">
         <v>23</v>
       </c>
@@ -1427,7 +1439,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I39" s="9" t="s">
         <v>4</v>
       </c>
@@ -1435,7 +1447,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I40" s="9" t="s">
         <v>42</v>
       </c>
@@ -1443,7 +1455,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I41" s="9" t="s">
         <v>43</v>
       </c>
@@ -1451,7 +1463,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I42" s="12" t="s">
         <v>5</v>
       </c>
@@ -1474,16 +1486,16 @@
       <selection pane="bottomLeft" activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="12.7109375" style="6" customWidth="1"/>
+    <col min="1" max="3" width="12.6640625" style="6" customWidth="1"/>
     <col min="4" max="4" width="20" style="6" customWidth="1"/>
-    <col min="5" max="5" width="88.42578125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="6" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="6"/>
+    <col min="5" max="5" width="88.44140625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="6" customWidth="1"/>
+    <col min="7" max="16384" width="11.44140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -1503,7 +1515,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="4" customFormat="1" ht="300" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="4" customFormat="1" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
       <c r="B2" s="15" t="s">
         <v>68</v>
@@ -1521,7 +1533,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
@@ -1529,7 +1541,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="2"/>
@@ -1537,7 +1549,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="2"/>
@@ -1545,7 +1557,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="2"/>
@@ -1553,7 +1565,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
@@ -1561,7 +1573,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="2"/>
@@ -1569,7 +1581,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="2"/>
@@ -1577,7 +1589,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="2"/>
@@ -1585,7 +1597,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
@@ -1593,7 +1605,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
@@ -1601,7 +1613,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
@@ -1609,7 +1621,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
@@ -1617,7 +1629,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2"/>
@@ -1625,7 +1637,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="2"/>
@@ -1633,7 +1645,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="2"/>
@@ -1641,7 +1653,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="2"/>
@@ -1649,7 +1661,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="2"/>
@@ -1657,7 +1669,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="2"/>
@@ -1665,7 +1677,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="2"/>
@@ -1673,7 +1685,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="2"/>
@@ -1681,7 +1693,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="2"/>
@@ -1705,15 +1717,15 @@
       <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="12.7109375" style="6" customWidth="1"/>
-    <col min="5" max="7" width="32.42578125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="6" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="6"/>
+    <col min="1" max="4" width="12.6640625" style="6" customWidth="1"/>
+    <col min="5" max="7" width="32.44140625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="6" customWidth="1"/>
+    <col min="9" max="16384" width="11.44140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -1730,7 +1742,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G1" s="23" t="s">
         <v>26</v>
@@ -1739,7 +1751,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A2" s="20"/>
       <c r="B2" s="21" t="s">
         <v>67</v>
@@ -1749,129 +1761,129 @@
         <v>66</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H2" s="20" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A3" s="18"/>
       <c r="B3" s="21" t="s">
         <v>67</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H3" s="18" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A4" s="18"/>
       <c r="B4" s="21" t="s">
         <v>67</v>
       </c>
       <c r="C4" s="19"/>
       <c r="D4" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H4" s="18" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A5" s="18"/>
       <c r="B5" s="21" t="s">
         <v>67</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H5" s="18" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A6" s="18"/>
       <c r="B6" s="21" t="s">
         <v>67</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H6" s="18" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A7" s="18"/>
       <c r="B7" s="21" t="s">
         <v>67</v>
       </c>
       <c r="C7" s="19"/>
       <c r="D7" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H7" s="18" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="18"/>
       <c r="B8" s="19"/>
       <c r="C8" s="19"/>
@@ -1881,7 +1893,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="18"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="18"/>
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
@@ -1891,7 +1903,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="18"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="18"/>
       <c r="B10" s="19"/>
       <c r="C10" s="19"/>
@@ -1901,7 +1913,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="18"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
       <c r="B11" s="19"/>
       <c r="C11" s="19"/>
@@ -1911,7 +1923,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="18"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
@@ -1921,7 +1933,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="18"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="19"/>
       <c r="C13" s="19"/>
@@ -1931,7 +1943,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="18"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="18"/>
       <c r="B14" s="19"/>
       <c r="C14" s="19"/>
@@ -1941,7 +1953,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="18"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="18"/>
       <c r="B15" s="19"/>
       <c r="C15" s="19"/>
@@ -1951,7 +1963,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="18"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
       <c r="B16" s="19"/>
       <c r="C16" s="19"/>
@@ -1961,7 +1973,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="18"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="18"/>
       <c r="B17" s="19"/>
       <c r="C17" s="19"/>
@@ -1971,7 +1983,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="18"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="18"/>
       <c r="B18" s="19"/>
       <c r="C18" s="19"/>
@@ -1981,7 +1993,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="18"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="18"/>
       <c r="B19" s="19"/>
       <c r="C19" s="19"/>
@@ -1991,7 +2003,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="18"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="18"/>
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
@@ -2001,7 +2013,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="18"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="18"/>
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
@@ -2026,16 +2038,16 @@
       <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="12.7109375" style="6" customWidth="1"/>
-    <col min="3" max="4" width="31.42578125" style="6" customWidth="1"/>
+    <col min="1" max="2" width="12.6640625" style="6" customWidth="1"/>
+    <col min="3" max="4" width="31.44140625" style="6" customWidth="1"/>
     <col min="5" max="5" width="36" style="6" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="6" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="6"/>
+    <col min="6" max="6" width="12.6640625" style="6" customWidth="1"/>
+    <col min="7" max="16384" width="11.44140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -2055,77 +2067,77 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="360" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A2" s="20"/>
       <c r="B2" s="20"/>
       <c r="C2" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="E2" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="E2" s="16" t="s">
-        <v>103</v>
-      </c>
       <c r="F2" s="20"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="18"/>
       <c r="B3" s="18"/>
       <c r="C3" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="E3" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="E3" s="19" t="s">
-        <v>106</v>
-      </c>
       <c r="F3" s="18"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="18"/>
       <c r="B4" s="18"/>
       <c r="C4" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="E4" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="E4" s="19" t="s">
-        <v>109</v>
-      </c>
       <c r="F4" s="18"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="18"/>
       <c r="B5" s="18"/>
       <c r="C5" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="E5" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="E5" s="19" t="s">
-        <v>112</v>
-      </c>
       <c r="F5" s="18"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="18"/>
       <c r="B6" s="18"/>
       <c r="C6" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="D6" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="E6" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="E6" s="19" t="s">
-        <v>115</v>
-      </c>
       <c r="F6" s="18"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="18"/>
       <c r="B7" s="18"/>
       <c r="C7" s="19"/>
@@ -2133,7 +2145,7 @@
       <c r="E7" s="19"/>
       <c r="F7" s="18"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="18"/>
       <c r="B8" s="18"/>
       <c r="C8" s="19"/>
@@ -2141,7 +2153,7 @@
       <c r="E8" s="19"/>
       <c r="F8" s="18"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="18"/>
       <c r="B9" s="18"/>
       <c r="C9" s="19"/>
@@ -2149,7 +2161,7 @@
       <c r="E9" s="19"/>
       <c r="F9" s="18"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="18"/>
       <c r="B10" s="18"/>
       <c r="C10" s="19"/>
@@ -2157,7 +2169,7 @@
       <c r="E10" s="19"/>
       <c r="F10" s="18"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
       <c r="B11" s="18"/>
       <c r="C11" s="19"/>
@@ -2165,7 +2177,7 @@
       <c r="E11" s="19"/>
       <c r="F11" s="18"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
       <c r="B12" s="18"/>
       <c r="C12" s="19"/>
@@ -2173,7 +2185,7 @@
       <c r="E12" s="19"/>
       <c r="F12" s="18"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="18"/>
       <c r="C13" s="19"/>
@@ -2181,7 +2193,7 @@
       <c r="E13" s="19"/>
       <c r="F13" s="18"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="18"/>
       <c r="B14" s="18"/>
       <c r="C14" s="19"/>
@@ -2189,7 +2201,7 @@
       <c r="E14" s="19"/>
       <c r="F14" s="18"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="18"/>
       <c r="B15" s="18"/>
       <c r="C15" s="19"/>
@@ -2197,7 +2209,7 @@
       <c r="E15" s="19"/>
       <c r="F15" s="18"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
       <c r="B16" s="18"/>
       <c r="C16" s="19"/>
@@ -2205,7 +2217,7 @@
       <c r="E16" s="19"/>
       <c r="F16" s="18"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="18"/>
       <c r="B17" s="18"/>
       <c r="C17" s="19"/>
@@ -2213,7 +2225,7 @@
       <c r="E17" s="19"/>
       <c r="F17" s="18"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="18"/>
       <c r="B18" s="18"/>
       <c r="C18" s="19"/>
@@ -2221,7 +2233,7 @@
       <c r="E18" s="19"/>
       <c r="F18" s="18"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="18"/>
       <c r="B19" s="18"/>
       <c r="C19" s="19"/>
@@ -2229,7 +2241,7 @@
       <c r="E19" s="19"/>
       <c r="F19" s="18"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="18"/>
       <c r="B20" s="18"/>
       <c r="C20" s="19"/>
@@ -2237,7 +2249,7 @@
       <c r="E20" s="19"/>
       <c r="F20" s="18"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="18"/>
       <c r="B21" s="18"/>
       <c r="C21" s="19"/>
@@ -2245,7 +2257,7 @@
       <c r="E21" s="19"/>
       <c r="F21" s="18"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="18"/>
       <c r="B22" s="18"/>
       <c r="C22" s="19"/>
@@ -2253,7 +2265,7 @@
       <c r="E22" s="19"/>
       <c r="F22" s="18"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="18"/>
       <c r="B23" s="18"/>
       <c r="C23" s="19"/>
@@ -2261,7 +2273,7 @@
       <c r="E23" s="19"/>
       <c r="F23" s="18"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="18"/>
       <c r="B24" s="18"/>
       <c r="C24" s="19"/>
@@ -2269,7 +2281,7 @@
       <c r="E24" s="19"/>
       <c r="F24" s="18"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="18"/>
       <c r="B25" s="18"/>
       <c r="C25" s="19"/>
@@ -2297,16 +2309,16 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="41.140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="6"/>
+    <col min="1" max="1" width="12.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="41.109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="11.44140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -2320,7 +2332,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>68</v>
       </c>
@@ -2334,7 +2346,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>69</v>
       </c>
@@ -2348,79 +2360,79 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="18"/>
       <c r="B4" s="19"/>
       <c r="C4" s="19"/>
       <c r="D4" s="18"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="18"/>
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
       <c r="D5" s="18"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="18"/>
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
       <c r="D6" s="18"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="18"/>
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
       <c r="D7" s="18"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="18"/>
       <c r="B8" s="19"/>
       <c r="C8" s="19"/>
       <c r="D8" s="18"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="18"/>
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
       <c r="D9" s="18"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="18"/>
       <c r="B10" s="19"/>
       <c r="C10" s="19"/>
       <c r="D10" s="18"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
       <c r="B11" s="19"/>
       <c r="C11" s="19"/>
       <c r="D11" s="18"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
       <c r="D12" s="18"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="19"/>
       <c r="C13" s="19"/>
       <c r="D13" s="18"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="18"/>
       <c r="B14" s="19"/>
       <c r="C14" s="19"/>
       <c r="D14" s="18"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="18"/>
       <c r="B15" s="19"/>
       <c r="C15" s="19"/>
       <c r="D15" s="18"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
       <c r="B16" s="19"/>
       <c r="C16" s="19"/>
@@ -2438,20 +2450,20 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1:B1048576"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="12.7109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" style="6" customWidth="1"/>
+    <col min="1" max="2" width="12.6640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="29.109375" style="6" customWidth="1"/>
     <col min="4" max="4" width="31" style="4" customWidth="1"/>
-    <col min="5" max="5" width="50.140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="6" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="6"/>
+    <col min="5" max="5" width="50.109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="6" customWidth="1"/>
+    <col min="7" max="16384" width="11.44140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -2471,7 +2483,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="20"/>
       <c r="B2" s="20" t="s">
         <v>69</v>
@@ -2483,35 +2495,45 @@
         <v>74</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="F2" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="18"/>
       <c r="B3" s="18"/>
       <c r="C3" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>118</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F3" s="18"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="F3" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="18"/>
       <c r="B4" s="18"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="18"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C4" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F4" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="18"/>
       <c r="B5" s="18"/>
       <c r="C5" s="19"/>
@@ -2519,7 +2541,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="18"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="18"/>
       <c r="B6" s="18"/>
       <c r="C6" s="19"/>
@@ -2527,7 +2549,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="18"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="18"/>
       <c r="B7" s="18"/>
       <c r="C7" s="19"/>
@@ -2535,7 +2557,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="18"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="18"/>
       <c r="B8" s="18"/>
       <c r="C8" s="19"/>
@@ -2543,7 +2565,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="18"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="18"/>
       <c r="B9" s="18"/>
       <c r="C9" s="19"/>
@@ -2551,7 +2573,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="18"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="18"/>
       <c r="B10" s="18"/>
       <c r="C10" s="19"/>
@@ -2559,7 +2581,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="18"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
       <c r="B11" s="18"/>
       <c r="C11" s="19"/>
@@ -2567,7 +2589,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="18"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
       <c r="B12" s="18"/>
       <c r="C12" s="19"/>
@@ -2575,7 +2597,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="18"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="18"/>
       <c r="C13" s="19"/>
@@ -2583,7 +2605,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="18"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="18"/>
       <c r="B14" s="18"/>
       <c r="C14" s="19"/>
@@ -2591,7 +2613,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="18"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="18"/>
       <c r="B15" s="18"/>
       <c r="C15" s="19"/>
@@ -2599,7 +2621,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="18"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
       <c r="B16" s="18"/>
       <c r="C16" s="19"/>
@@ -2607,7 +2629,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="18"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="18"/>
       <c r="B17" s="18"/>
       <c r="C17" s="19"/>
@@ -2615,7 +2637,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="18"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="18"/>
       <c r="B18" s="18"/>
       <c r="C18" s="19"/>
@@ -2636,24 +2658,25 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1:B1048576"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="6" customWidth="1"/>
-    <col min="2" max="3" width="11.42578125" style="6"/>
+    <col min="1" max="1" width="12.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" style="6"/>
     <col min="4" max="4" width="29" style="6" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="6"/>
+    <col min="5" max="5" width="12.6640625" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="11.44140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>32</v>
+        <v>130</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>36</v>
@@ -2665,150 +2688,150 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="20"/>
       <c r="B2" s="21" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C2" s="21"/>
       <c r="D2" s="21" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E2" s="20">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="18"/>
       <c r="B3" s="19" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="19" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E3" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="18"/>
       <c r="B4" s="19" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C4" s="19"/>
       <c r="D4" s="19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E4" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="18"/>
       <c r="B5" s="19" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="19" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E5" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="18"/>
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
       <c r="E6" s="18"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="18"/>
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
       <c r="D7" s="19"/>
       <c r="E7" s="18"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="18"/>
       <c r="B8" s="19"/>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
       <c r="E8" s="18"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="18"/>
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
       <c r="D9" s="19"/>
       <c r="E9" s="18"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="18"/>
       <c r="B10" s="19"/>
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
       <c r="E10" s="18"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
       <c r="B11" s="19"/>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
       <c r="E11" s="18"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
       <c r="D12" s="19"/>
       <c r="E12" s="18"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="19"/>
       <c r="C13" s="19"/>
       <c r="D13" s="19"/>
       <c r="E13" s="18"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="18"/>
       <c r="B14" s="19"/>
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
       <c r="E14" s="18"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="18"/>
       <c r="B15" s="19"/>
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
       <c r="E15" s="18"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
       <c r="B16" s="19"/>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
       <c r="E16" s="18"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="18"/>
       <c r="B17" s="19"/>
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
       <c r="E17" s="18"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="18"/>
       <c r="B18" s="19"/>
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
       <c r="E18" s="18"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="18"/>
       <c r="B19" s="19"/>
       <c r="C19" s="19"/>
@@ -2824,24 +2847,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1:B1048576"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="12.7109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="33.7109375" style="6" customWidth="1"/>
+    <col min="1" max="2" width="12.6640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="33.6640625" style="6" customWidth="1"/>
     <col min="6" max="6" width="38" style="6" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="6" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="6"/>
+    <col min="7" max="7" width="12.6640625" style="6" customWidth="1"/>
+    <col min="8" max="16384" width="11.44140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -2864,7 +2887,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="22" t="s">
@@ -2881,7 +2904,7 @@
       </c>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="285" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="3" t="s">
@@ -2898,7 +2921,7 @@
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="144" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="3" t="s">
@@ -2915,7 +2938,7 @@
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="240" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="3" t="s">
@@ -2932,7 +2955,7 @@
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="210" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="3"/>

</xml_diff>